<commit_message>
Deleting Leaves and whole Tree
</commit_message>
<xml_diff>
--- a/ProblemsAndSolution.xlsx
+++ b/ProblemsAndSolution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Problem</t>
   </si>
@@ -189,13 +189,19 @@
     <t>https://gist.github.com/baranis/64fc3cd71b01d109d638</t>
   </si>
   <si>
+    <t>https://gist.github.com/baranis/927e23530db540e8ae06</t>
+  </si>
+  <si>
+    <t>Delete all leaves in a tree</t>
+  </si>
+  <si>
+    <t>http://ideone.com/gv4dZS</t>
+  </si>
+  <si>
+    <t>Delete Tree</t>
+  </si>
+  <si>
     <t>http://ideone.com/g23yCk</t>
-  </si>
-  <si>
-    <t>https://gist.github.com/baranis/927e23530db540e8ae06</t>
-  </si>
-  <si>
-    <t>Delete all leaves in a tree</t>
   </si>
 </sst>
 </file>
@@ -560,11 +566,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,20 +809,27 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>57</v>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="A10" r:id="rId2" display="https://gist.github.com/baranis/c027031b1505227abd21"/>
-    <hyperlink ref="C29" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Started after so much so struggle and patience ... Mankatha da..
</commit_message>
<xml_diff>
--- a/ProblemsAndSolution.xlsx
+++ b/ProblemsAndSolution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Problem</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Given a binary tree, change the right pointer of every leaf node to the next leaf node (right to it but may be on different level).</t>
+  </si>
+  <si>
+    <t>http://ideone.com/KDIRqw</t>
   </si>
 </sst>
 </file>
@@ -678,8 +681,8 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,6 +780,9 @@
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1031,9 +1037,10 @@
     <hyperlink ref="C3" r:id="rId6"/>
     <hyperlink ref="B36" r:id="rId7"/>
     <hyperlink ref="B39" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated With My Changes
</commit_message>
<xml_diff>
--- a/ProblemsAndSolution.xlsx
+++ b/ProblemsAndSolution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Problem</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>http://ideone.com/KDIRqw</t>
+  </si>
+  <si>
+    <t>http://ideone.com/mk12Vi</t>
   </si>
 </sst>
 </file>
@@ -681,8 +684,8 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +966,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
@@ -971,7 +974,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>70</v>
       </c>
@@ -979,15 +982,18 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>74</v>
       </c>
@@ -995,7 +1001,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>77</v>
       </c>
@@ -1003,7 +1009,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>78</v>
       </c>
@@ -1011,7 +1017,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>81</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>83</v>
       </c>
@@ -1038,9 +1044,10 @@
     <hyperlink ref="B36" r:id="rId7"/>
     <hyperlink ref="B39" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C35" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated with so much pain..
</commit_message>
<xml_diff>
--- a/ProblemsAndSolution.xlsx
+++ b/ProblemsAndSolution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="420" windowWidth="21075" windowHeight="9735"/>
+    <workbookView xWindow="240" yWindow="420" windowWidth="20700" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Problem</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>https://gist.github.com/baranis/53a12914a51782a4836d</t>
+  </si>
+  <si>
+    <t>http://ideone.com/jPggDs</t>
   </si>
 </sst>
 </file>
@@ -711,8 +714,8 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,6 +764,9 @@
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated with huge stress
</commit_message>
<xml_diff>
--- a/ProblemsAndSolution.xlsx
+++ b/ProblemsAndSolution.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="480" windowWidth="20700" windowHeight="9675"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Problem</t>
   </si>
@@ -386,12 +386,15 @@
   <si>
     <t>https://gist.github.com/baranis/a7979b20b41ed458186b</t>
   </si>
+  <si>
+    <t>http://ideone.com/TAXHIA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,7 +554,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -586,7 +588,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -762,22 +763,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="75" style="3" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -788,7 +789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -799,7 +800,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="45">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -810,7 +811,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -821,7 +822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="45">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -829,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -837,7 +838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -845,7 +846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="45">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -853,15 +854,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -872,7 +876,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="30">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -880,7 +884,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="45">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -888,7 +892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -896,7 +900,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="45">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -904,7 +908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="45">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -912,7 +916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
@@ -920,7 +924,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
@@ -928,7 +932,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="45">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
@@ -936,7 +940,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
@@ -944,7 +948,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -952,7 +956,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -960,7 +964,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -968,7 +972,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
         <v>46</v>
       </c>
@@ -976,7 +980,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
         <v>47</v>
       </c>
@@ -984,7 +988,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -992,7 +996,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
         <v>51</v>
       </c>
@@ -1000,7 +1004,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
         <v>53</v>
       </c>
@@ -1008,7 +1012,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
         <v>55</v>
       </c>
@@ -1016,7 +1020,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
         <v>58</v>
       </c>
@@ -1027,7 +1031,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
         <v>59</v>
       </c>
@@ -1035,7 +1039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
         <v>62</v>
       </c>
@@ -1043,7 +1047,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="30">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -1051,7 +1055,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="45">
       <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
@@ -1059,7 +1063,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="105">
       <c r="A34" s="3" t="s">
         <v>70</v>
       </c>
@@ -1067,7 +1071,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="3" t="s">
         <v>73</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="105">
       <c r="A36" s="3" t="s">
         <v>74</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="120">
       <c r="A37" s="3" t="s">
         <v>77</v>
       </c>
@@ -1094,7 +1098,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="315">
       <c r="A38" s="3" t="s">
         <v>78</v>
       </c>
@@ -1102,7 +1106,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="60">
       <c r="A39" s="3" t="s">
         <v>81</v>
       </c>
@@ -1110,7 +1114,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="30">
       <c r="A40" s="3" t="s">
         <v>83</v>
       </c>
@@ -1118,7 +1122,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="195">
       <c r="A41" s="3" t="s">
         <v>86</v>
       </c>
@@ -1126,7 +1130,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="150">
       <c r="A42" s="3" t="s">
         <v>88</v>
       </c>
@@ -1134,7 +1138,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
@@ -1142,7 +1146,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="120">
       <c r="A44" s="3" t="s">
         <v>93</v>
       </c>
@@ -1150,7 +1154,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="60">
       <c r="A45" s="3" t="s">
         <v>95</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="3" t="s">
         <v>97</v>
       </c>
@@ -1166,7 +1170,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="195">
       <c r="A47" s="3" t="s">
         <v>99</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="30">
       <c r="A48" s="3" t="s">
         <v>101</v>
       </c>
@@ -1203,24 +1207,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
solved some of problems
</commit_message>
<xml_diff>
--- a/ProblemsAndSolution.xlsx
+++ b/ProblemsAndSolution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Problem</t>
   </si>
@@ -411,6 +411,9 @@
   </si>
   <si>
     <t>http://ideone.com/Y2V2kV</t>
+  </si>
+  <si>
+    <t>http://ideone.com/bbbXHe</t>
   </si>
 </sst>
 </file>
@@ -790,8 +793,8 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1079,6 +1082,9 @@
       </c>
       <c r="B32" s="2" t="s">
         <v>66</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="45">

</xml_diff>

<commit_message>
Updated with So much grace.
</commit_message>
<xml_diff>
--- a/ProblemsAndSolution.xlsx
+++ b/ProblemsAndSolution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Problem</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>http://ideone.com/Vbiswh</t>
+  </si>
+  <si>
+    <t>http://ideone.com/WO7xJW</t>
   </si>
 </sst>
 </file>
@@ -797,7 +800,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1045,6 +1048,9 @@
       </c>
       <c r="B27" s="2" t="s">
         <v>54</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:3">

</xml_diff>

<commit_message>
Updated Track Of Sarath.xlsx and ProblemsAndSolution.xlsx
</commit_message>
<xml_diff>
--- a/ProblemsAndSolution.xlsx
+++ b/ProblemsAndSolution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="259">
   <si>
     <t>Problem</t>
   </si>
@@ -952,22 +952,16 @@
     <t>https://gist.github.com/baranis/718f51bb7251cb1c0a63</t>
   </si>
   <si>
-    <t>Print all nodes that are at distance k from a leaf node</t>
-  </si>
-  <si>
-    <t>https://gist.github.com/baranis/3f06f159aacc49697fac</t>
-  </si>
-  <si>
-    <t>ReverseEveryKNodes</t>
-  </si>
-  <si>
-    <t>https://gist.github.com/baranis/1ba89234698fbe642e04</t>
-  </si>
-  <si>
-    <t>GetAllUniqueNodesKDistanceFromRoot</t>
-  </si>
-  <si>
-    <t>https://gist.github.com/baranis/b8d75d53c53734176d2e</t>
+    <t>http://ideone.com/ymyLOU</t>
+  </si>
+  <si>
+    <t>UniqueNodes at K Distance From Root,Assuming No Duplicate Values at Nodes</t>
+  </si>
+  <si>
+    <t>Reverse Every K Nodes in Linked List</t>
+  </si>
+  <si>
+    <t>http://ideone.com/25I7AF</t>
   </si>
 </sst>
 </file>
@@ -1363,11 +1357,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A124" sqref="A124"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2384,26 +2378,18 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -2427,9 +2413,11 @@
     <hyperlink ref="C37" r:id="rId17"/>
     <hyperlink ref="C115" r:id="rId18"/>
     <hyperlink ref="C116" r:id="rId19"/>
+    <hyperlink ref="C121" r:id="rId20"/>
+    <hyperlink ref="C122" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Solutions Completed and Added.
</commit_message>
<xml_diff>
--- a/ProblemsAndSolution.xlsx
+++ b/ProblemsAndSolution.xlsx
@@ -15,6 +15,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>WIN764BIT</author>
+  </authors>
+  <commentList>
+    <comment ref="B122" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>WIN764BIT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Review Pending by sarath
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C122" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>WIN764BIT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Reverse nodes in single parse
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="263">
   <si>
@@ -980,7 +1040,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1016,6 +1076,19 @@
       <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1368,12 +1441,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
+      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,6 +2517,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId22"/>
+  <legacyDrawing r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>